<commit_message>
Before Poland update - have a semi-working model
</commit_message>
<xml_diff>
--- a/documentation/models.xlsx
+++ b/documentation/models.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming\Deep-Sudoku\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC37173-2FB9-480C-8B5E-DF28017C74FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B02E3441-A0DA-49D1-9CB8-02BF2DA56F4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31725" yWindow="7830" windowWidth="23280" windowHeight="13365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4140" yWindow="1425" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Number</t>
   </si>
@@ -34,12 +34,6 @@
   </si>
   <si>
     <t>Loss</t>
-  </si>
-  <si>
-    <t>6 convolutional layers, 64 hidden channels</t>
-  </si>
-  <si>
-    <t>10 convolutional layers, 128 hidden channels</t>
   </si>
 </sst>
 </file>
@@ -357,10 +351,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -379,25 +373,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1.66</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>